<commit_message>
Netzplan Übung 3 FIAE D ++
</commit_message>
<xml_diff>
--- a/FIAED Übungen/Netzplan_Übung_3.xlsx
+++ b/FIAED Übungen/Netzplan_Übung_3.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="16">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -60,6 +61,15 @@
   <si>
     <t xml:space="preserve">I</t>
   </si>
+  <si>
+    <t xml:space="preserve">B,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E,F</t>
+  </si>
 </sst>
 </file>
 
@@ -69,7 +79,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -109,8 +119,14 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,8 +151,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -172,6 +200,27 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -198,7 +247,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,7 +272,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,16 +308,44 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -304,7 +381,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -329,7 +406,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1154,7 +1231,7 @@
   <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y9" activeCellId="0" sqref="Y9"/>
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1180,17 +1257,28 @@
         <v>0</v>
       </c>
       <c r="K1" s="5"/>
-      <c r="L1" s="6"/>
+      <c r="L1" s="6" t="n">
+        <f aca="false">J1+J3</f>
+        <v>6</v>
+      </c>
       <c r="O1" s="4" t="n">
-        <v>0</v>
+        <f aca="false">L1</f>
+        <v>6</v>
       </c>
       <c r="P1" s="5"/>
-      <c r="Q1" s="6"/>
+      <c r="Q1" s="6" t="n">
+        <f aca="false">O1+O3</f>
+        <v>10</v>
+      </c>
       <c r="Y1" s="4" t="n">
-        <v>0</v>
+        <f aca="false">MAX(Q1,V7)</f>
+        <v>13</v>
       </c>
       <c r="Z1" s="5"/>
-      <c r="AA1" s="6"/>
+      <c r="AA1" s="6" t="n">
+        <f aca="false">Y1+Y3</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -1250,20 +1338,38 @@
         <f aca="false">H2</f>
         <v>6</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="K3" s="15" t="n">
+        <f aca="false">L4-L1</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="15" t="n">
+        <f aca="false">MIN(O1,O7,O13)-L1</f>
+        <v>0</v>
+      </c>
       <c r="O3" s="14" t="n">
         <f aca="false">H3</f>
         <v>4</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
+      <c r="P3" s="15" t="n">
+        <f aca="false">Q4-Q1</f>
+        <v>3</v>
+      </c>
+      <c r="Q3" s="15" t="n">
+        <f aca="false">Y1-Q1</f>
+        <v>3</v>
+      </c>
       <c r="Y3" s="14" t="n">
         <f aca="false">H8</f>
         <v>1</v>
       </c>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
+      <c r="Z3" s="15" t="n">
+        <f aca="false">AA4-AA1</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="15" t="n">
+        <f aca="false">AD7-AA1</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1282,15 +1388,33 @@
       <c r="H4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J4" s="16"/>
+      <c r="J4" s="16" t="n">
+        <f aca="false">L4-J3</f>
+        <v>0</v>
+      </c>
       <c r="K4" s="5"/>
-      <c r="L4" s="17"/>
-      <c r="O4" s="16"/>
+      <c r="L4" s="17" t="n">
+        <f aca="false">MIN(O4,O10,O17)</f>
+        <v>6</v>
+      </c>
+      <c r="O4" s="16" t="n">
+        <f aca="false">Q4-O3</f>
+        <v>9</v>
+      </c>
       <c r="P4" s="5"/>
-      <c r="Q4" s="17"/>
-      <c r="Y4" s="16"/>
+      <c r="Q4" s="17" t="n">
+        <f aca="false">Y4</f>
+        <v>13</v>
+      </c>
+      <c r="Y4" s="16" t="n">
+        <f aca="false">AA4-Y3</f>
+        <v>13</v>
+      </c>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="17"/>
+      <c r="AA4" s="17" t="n">
+        <f aca="false">AD10</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -1346,20 +1470,32 @@
         <v>2</v>
       </c>
       <c r="O7" s="4" t="n">
-        <v>0</v>
+        <f aca="false">L1</f>
+        <v>6</v>
       </c>
       <c r="P7" s="5"/>
-      <c r="Q7" s="6"/>
+      <c r="Q7" s="6" t="n">
+        <f aca="false">O7+O9</f>
+        <v>11</v>
+      </c>
       <c r="T7" s="4" t="n">
-        <v>0</v>
+        <f aca="false">Q7</f>
+        <v>11</v>
       </c>
       <c r="U7" s="5"/>
-      <c r="V7" s="6"/>
+      <c r="V7" s="6" t="n">
+        <f aca="false">T7+T9</f>
+        <v>13</v>
+      </c>
       <c r="AD7" s="4" t="n">
-        <v>0</v>
+        <f aca="false">MAX(AA1,AA13)</f>
+        <v>14</v>
       </c>
       <c r="AE7" s="5"/>
-      <c r="AF7" s="6"/>
+      <c r="AF7" s="6" t="n">
+        <f aca="false">AD7+AD9</f>
+        <v>23</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -1417,19 +1553,34 @@
         <f aca="false">H5</f>
         <v>5</v>
       </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
+      <c r="P9" s="15" t="n">
+        <f aca="false">Q10-Q7</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="15" t="n">
+        <f aca="false">T7-Q7</f>
+        <v>0</v>
+      </c>
       <c r="T9" s="14" t="n">
         <f aca="false">H7</f>
         <v>2</v>
       </c>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
+      <c r="U9" s="15" t="n">
+        <f aca="false">V10-V7</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="15" t="n">
+        <f aca="false">Y1-V7</f>
+        <v>0</v>
+      </c>
       <c r="AD9" s="14" t="n">
         <f aca="false">H10</f>
         <v>9</v>
       </c>
-      <c r="AE9" s="15"/>
+      <c r="AE9" s="15" t="n">
+        <f aca="false">AF10-AF7</f>
+        <v>0</v>
+      </c>
       <c r="AF9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,32 +1600,62 @@
       <c r="H10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="O10" s="16"/>
+      <c r="O10" s="16" t="n">
+        <f aca="false">Q10-O9</f>
+        <v>6</v>
+      </c>
       <c r="P10" s="5"/>
-      <c r="Q10" s="17"/>
-      <c r="T10" s="16"/>
+      <c r="Q10" s="17" t="n">
+        <f aca="false">T10</f>
+        <v>11</v>
+      </c>
+      <c r="T10" s="16" t="n">
+        <f aca="false">V10-T9</f>
+        <v>11</v>
+      </c>
       <c r="U10" s="5"/>
-      <c r="V10" s="17"/>
-      <c r="AD10" s="16"/>
+      <c r="V10" s="17" t="n">
+        <f aca="false">Y4</f>
+        <v>13</v>
+      </c>
+      <c r="AD10" s="16" t="n">
+        <f aca="false">AF10-AD9</f>
+        <v>14</v>
+      </c>
       <c r="AE10" s="5"/>
-      <c r="AF10" s="17"/>
+      <c r="AF10" s="17" t="n">
+        <f aca="false">AF7</f>
+        <v>23</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O13" s="4" t="n">
-        <v>0</v>
+        <f aca="false">L1</f>
+        <v>6</v>
       </c>
       <c r="P13" s="5"/>
-      <c r="Q13" s="6"/>
+      <c r="Q13" s="6" t="n">
+        <f aca="false">O13+O15</f>
+        <v>9</v>
+      </c>
       <c r="T13" s="4" t="n">
-        <v>0</v>
+        <f aca="false">Q13</f>
+        <v>9</v>
       </c>
       <c r="U13" s="5"/>
-      <c r="V13" s="6"/>
+      <c r="V13" s="6" t="n">
+        <f aca="false">T13+T15</f>
+        <v>12</v>
+      </c>
       <c r="Y13" s="4" t="n">
-        <v>0</v>
+        <f aca="false">V13</f>
+        <v>12</v>
       </c>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="6"/>
+      <c r="AA13" s="6" t="n">
+        <f aca="false">Y13+Y15</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O14" s="11" t="s">
@@ -1498,31 +1679,67 @@
         <f aca="false">H4</f>
         <v>3</v>
       </c>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
+      <c r="P15" s="15" t="n">
+        <f aca="false">Q16-Q13</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="15" t="n">
+        <f aca="false">T13-Q13</f>
+        <v>0</v>
+      </c>
       <c r="T15" s="14" t="n">
         <f aca="false">H6</f>
         <v>3</v>
       </c>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
+      <c r="U15" s="15" t="n">
+        <f aca="false">V16-V13</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="15" t="n">
+        <f aca="false">Y13-V13</f>
+        <v>0</v>
+      </c>
       <c r="Y15" s="14" t="n">
         <f aca="false">H9</f>
         <v>2</v>
       </c>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
+      <c r="Z15" s="15" t="n">
+        <f aca="false">AA16-AA13</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="15" t="n">
+        <f aca="false">AD7-AA13</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O16" s="16"/>
+      <c r="O16" s="16" t="n">
+        <f aca="false">Q16-O15</f>
+        <v>6</v>
+      </c>
       <c r="P16" s="5"/>
-      <c r="Q16" s="17"/>
-      <c r="T16" s="16"/>
+      <c r="Q16" s="17" t="n">
+        <f aca="false">T16</f>
+        <v>9</v>
+      </c>
+      <c r="T16" s="16" t="n">
+        <f aca="false">V16-T15</f>
+        <v>9</v>
+      </c>
       <c r="U16" s="5"/>
-      <c r="V16" s="17"/>
-      <c r="Y16" s="16"/>
+      <c r="V16" s="17" t="n">
+        <f aca="false">Y16</f>
+        <v>12</v>
+      </c>
+      <c r="Y16" s="16" t="n">
+        <f aca="false">AA16-Y15</f>
+        <v>12</v>
+      </c>
       <c r="Z16" s="5"/>
-      <c r="AA16" s="17"/>
+      <c r="AA16" s="17" t="n">
+        <f aca="false">AD10</f>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1547,4 +1764,151 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="18" width="10.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="18" width="3.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="20" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="F3" s="14" t="n">
+        <f aca="false">D2</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Netzplan Übung 3 FIAE D Lösung
</commit_message>
<xml_diff>
--- a/FIAED Übungen/Netzplan_Übung_3.xlsx
+++ b/FIAED Übungen/Netzplan_Übung_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="16">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -357,11 +357,26 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="1"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1223,6 +1238,557 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3380400" y="325080"/>
+          <a:ext cx="0" cy="969480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>248040</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4456080" y="325080"/>
+          <a:ext cx="521280" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>267480</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>263880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5806440" y="325080"/>
+          <a:ext cx="266400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>268200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>249840</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7156440" y="1300320"/>
+          <a:ext cx="521280" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>269280</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>250560</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8506800" y="325080"/>
+          <a:ext cx="521280" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>264240</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3380400" y="1300320"/>
+          <a:ext cx="2962440" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>269280</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>265680</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8506800" y="1300320"/>
+          <a:ext cx="266400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>269280</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>258120</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8506800" y="1300320"/>
+          <a:ext cx="258840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>265680</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>246960</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3105720" y="325080"/>
+          <a:ext cx="521280" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>267480</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>267480</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076440" y="325440"/>
+          <a:ext cx="0" cy="969480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>269280</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>269280</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8776800" y="325440"/>
+          <a:ext cx="0" cy="969480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>268560</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7426800" y="325440"/>
+          <a:ext cx="0" cy="969480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>268920</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>258120</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7427160" y="325080"/>
+          <a:ext cx="258840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1230,8 +1796,8 @@
   </sheetPr>
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD19" activeCellId="0" sqref="AD19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE9" activeCellId="8" sqref="K3 P3 P9 P15 U9 U15 Z3 Z15 AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1755,6 +2321,11 @@
     <mergeCell ref="T14:V14"/>
     <mergeCell ref="Y14:AA14"/>
   </mergeCells>
+  <conditionalFormatting sqref="K3 P3 P9 P15 U9 U15 Z3 Z15 AE9">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1771,10 +2342,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:AG16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y11" activeCellId="9" sqref="K3 P3 P9 P15 U9 U15 Z3 Z15 AE9 Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1801,7 +2372,46 @@
         <v>0</v>
       </c>
       <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="H1" s="6" t="n">
+        <f aca="false">F1+F3</f>
+        <v>3</v>
+      </c>
+      <c r="K1" s="4" t="n">
+        <f aca="false">H1</f>
+        <v>3</v>
+      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="6" t="n">
+        <f aca="false">K1+K3</f>
+        <v>7</v>
+      </c>
+      <c r="P1" s="4" t="n">
+        <f aca="false">M1</f>
+        <v>7</v>
+      </c>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="6" t="n">
+        <f aca="false">P1+P3</f>
+        <v>10</v>
+      </c>
+      <c r="Z1" s="4" t="n">
+        <f aca="false">W7</f>
+        <v>12</v>
+      </c>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="6" t="n">
+        <f aca="false">Z1+Z3</f>
+        <v>21</v>
+      </c>
+      <c r="AE1" s="4" t="n">
+        <f aca="false">MAX(AB1,AB7)</f>
+        <v>21</v>
+      </c>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="6" t="n">
+        <f aca="false">AE1+AE3</f>
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
@@ -1819,6 +2429,26 @@
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
+      <c r="K2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="P2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="Z2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AE2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
@@ -1837,8 +2467,59 @@
         <f aca="false">D2</f>
         <v>3</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="G3" s="15" t="n">
+        <f aca="false">H4-H1</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="15" t="n">
+        <f aca="false">MIN(U7,K1)-H1</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="14" t="n">
+        <f aca="false">D3</f>
+        <v>4</v>
+      </c>
+      <c r="L3" s="15" t="n">
+        <f aca="false">M4-M1</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="15" t="n">
+        <f aca="false">P1-M1</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="14" t="n">
+        <f aca="false">D4</f>
+        <v>3</v>
+      </c>
+      <c r="Q3" s="15" t="n">
+        <f aca="false">R4-R1</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="15" t="n">
+        <f aca="false">U7-R1</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="14" t="n">
+        <f aca="false">D6</f>
+        <v>9</v>
+      </c>
+      <c r="AA3" s="15" t="n">
+        <f aca="false">AB4-AB1</f>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="15" t="n">
+        <f aca="false">AE1-AB1</f>
+        <v>0</v>
+      </c>
+      <c r="AE3" s="14" t="n">
+        <f aca="false">D8</f>
+        <v>6</v>
+      </c>
+      <c r="AF3" s="15" t="n">
+        <f aca="false">AG4-AG1</f>
+        <v>0</v>
+      </c>
+      <c r="AG3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
@@ -1853,9 +2534,51 @@
       <c r="D4" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="16" t="n">
+        <f aca="false">H4-F3</f>
+        <v>0</v>
+      </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="17"/>
+      <c r="H4" s="17" t="n">
+        <f aca="false">MIN(K4,U10)</f>
+        <v>3</v>
+      </c>
+      <c r="K4" s="16" t="n">
+        <f aca="false">M4-K3</f>
+        <v>3</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="17" t="n">
+        <f aca="false">P4</f>
+        <v>7</v>
+      </c>
+      <c r="P4" s="16" t="n">
+        <f aca="false">R4-P3</f>
+        <v>7</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="17" t="n">
+        <f aca="false">U10</f>
+        <v>10</v>
+      </c>
+      <c r="Z4" s="16" t="n">
+        <f aca="false">AB4-Z3</f>
+        <v>12</v>
+      </c>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="17" t="n">
+        <f aca="false">AE4</f>
+        <v>21</v>
+      </c>
+      <c r="AE4" s="16" t="n">
+        <f aca="false">AG4-AE3</f>
+        <v>21</v>
+      </c>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="17" t="n">
+        <f aca="false">AG1</f>
+        <v>27</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
@@ -1898,6 +2621,27 @@
       <c r="D7" s="22" t="n">
         <v>2</v>
       </c>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="U7" s="4" t="n">
+        <f aca="false">MAX(H1,R1)</f>
+        <v>10</v>
+      </c>
+      <c r="V7" s="5"/>
+      <c r="W7" s="6" t="n">
+        <f aca="false">U7+U9</f>
+        <v>12</v>
+      </c>
+      <c r="Z7" s="4" t="n">
+        <f aca="false">W7</f>
+        <v>12</v>
+      </c>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="6" t="n">
+        <f aca="false">Z7+Z9</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
@@ -1910,11 +2654,117 @@
       <c r="D8" s="23" t="n">
         <v>6</v>
       </c>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="U8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="Z8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="U9" s="14" t="n">
+        <f aca="false">D5</f>
+        <v>2</v>
+      </c>
+      <c r="V9" s="15" t="n">
+        <f aca="false">W10-W7</f>
+        <v>0</v>
+      </c>
+      <c r="W9" s="15" t="n">
+        <f aca="false">MIN(Z1,Z7)-W7</f>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="14" t="n">
+        <f aca="false">D7</f>
+        <v>2</v>
+      </c>
+      <c r="AA9" s="15" t="n">
+        <f aca="false">AB10-AB7</f>
+        <v>7</v>
+      </c>
+      <c r="AB9" s="15" t="n">
+        <f aca="false">AE1-AB7</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="U10" s="16" t="n">
+        <f aca="false">W10-U9</f>
+        <v>10</v>
+      </c>
+      <c r="V10" s="5"/>
+      <c r="W10" s="17" t="n">
+        <f aca="false">MIN(Z4,Z10)</f>
+        <v>12</v>
+      </c>
+      <c r="Z10" s="16" t="n">
+        <f aca="false">AB10-Z9</f>
+        <v>19</v>
+      </c>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="17" t="n">
+        <f aca="false">AE4</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z11" s="0"/>
+      <c r="AA11" s="0"/>
+      <c r="AB11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z12" s="0"/>
+      <c r="AA12" s="0"/>
+      <c r="AB12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z13" s="0"/>
+      <c r="AA13" s="0"/>
+      <c r="AB13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z14" s="0"/>
+      <c r="AA14" s="0"/>
+      <c r="AB14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z15" s="0"/>
+      <c r="AA15" s="0"/>
+      <c r="AB15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z16" s="0"/>
+      <c r="AA16" s="0"/>
+      <c r="AB16" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="7">
     <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="U8:W8"/>
+    <mergeCell ref="Z8:AB8"/>
   </mergeCells>
+  <conditionalFormatting sqref="G3 L3 Q3 V9 AA3 AA9 AF3">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1922,5 +2772,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lösung Ressourcen Netzpla_Übung 3 - FIAE D
</commit_message>
<xml_diff>
--- a/FIAED Übungen/Netzplan_Übung_3.xlsx
+++ b/FIAED Übungen/Netzplan_Übung_3.xlsx
@@ -84,15 +84,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0\ %"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,12 +110,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,6 +129,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -256,20 +253,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,7 +278,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,15 +290,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,15 +306,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,19 +322,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -337,11 +342,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -357,7 +370,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,10 +384,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -467,13 +480,13 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>264240</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>263880</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -482,40 +495,40 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4928760" y="319320"/>
-          <a:ext cx="539280" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="18000">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>212400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+          <a:off x="5149800" y="319680"/>
+          <a:ext cx="540720" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>258840</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>264960</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -523,9 +536,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5198760" y="325080"/>
-          <a:ext cx="0" cy="975240"/>
+        <a:xfrm>
+          <a:off x="5414400" y="325080"/>
+          <a:ext cx="6120" cy="966600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -549,13 +562,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>252000</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>258840</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
@@ -566,8 +579,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5186160" y="1302480"/>
-          <a:ext cx="276120" cy="0"/>
+          <a:off x="5408280" y="1301400"/>
+          <a:ext cx="276840" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -591,13 +604,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
@@ -608,50 +621,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5205240" y="2291400"/>
-          <a:ext cx="276120" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="18000">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>52920</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>218520</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5204880" y="1308600"/>
-          <a:ext cx="0" cy="975240"/>
+          <a:off x="5428080" y="2290320"/>
+          <a:ext cx="276840" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -675,7 +646,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
@@ -687,13 +658,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvPr id="4" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6283800" y="2291040"/>
-          <a:ext cx="539280" cy="0"/>
+          <a:off x="6508800" y="2289960"/>
+          <a:ext cx="539640" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -717,7 +688,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
@@ -729,13 +700,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvPr id="5" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7633440" y="2291040"/>
-          <a:ext cx="539280" cy="0"/>
+          <a:off x="7861680" y="2289960"/>
+          <a:ext cx="539640" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -759,25 +730,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>269280</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name=""/>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6283800" y="1308600"/>
-          <a:ext cx="539280" cy="0"/>
+          <a:off x="6508800" y="1307520"/>
+          <a:ext cx="539640" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -801,7 +772,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -813,13 +784,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvPr id="7" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6283800" y="325080"/>
-          <a:ext cx="539280" cy="0"/>
+          <a:off x="6508800" y="325080"/>
+          <a:ext cx="539640" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -843,7 +814,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -855,13 +826,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvPr id="8" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6823800" y="325080"/>
-          <a:ext cx="539280" cy="0"/>
+          <a:off x="7050240" y="325080"/>
+          <a:ext cx="539640" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -885,109 +856,67 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>270000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7363800" y="325080"/>
-          <a:ext cx="539280" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="18000">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>28</xdr:col>
       <xdr:colOff>720</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>270360</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name=""/>
+        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7591320" y="325080"/>
+          <a:ext cx="540000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>7560</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7903440" y="325080"/>
-          <a:ext cx="276120" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="18000">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>52200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>217800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7903080" y="325440"/>
-          <a:ext cx="0" cy="975240"/>
+          <a:off x="8132400" y="325080"/>
+          <a:ext cx="276840" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1011,7 +940,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:colOff>1440</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
@@ -1023,13 +952,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name=""/>
+        <xdr:cNvPr id="11" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7633800" y="1308240"/>
-          <a:ext cx="276120" cy="0"/>
+          <a:off x="7862400" y="1307160"/>
+          <a:ext cx="276480" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1053,25 +982,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name=""/>
+        <xdr:cNvPr id="12" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8983440" y="325080"/>
-          <a:ext cx="276120" cy="0"/>
+          <a:off x="9215280" y="325080"/>
+          <a:ext cx="276840" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1095,25 +1024,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>160560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name=""/>
+        <xdr:cNvPr id="13" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8983440" y="2291400"/>
-          <a:ext cx="276120" cy="0"/>
+          <a:off x="9215280" y="2290320"/>
+          <a:ext cx="276840" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1149,45 +1078,129 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9485280" y="1307160"/>
+          <a:ext cx="276480" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>6120</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>145800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5426280" y="1308600"/>
+          <a:ext cx="6120" cy="966600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
         <xdr:cNvPr id="16" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9253080" y="1308240"/>
-          <a:ext cx="276120" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="18000">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>52560</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>218160</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+        <a:xfrm>
+          <a:off x="8132040" y="326160"/>
+          <a:ext cx="6120" cy="966600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>6480</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1195,41 +1208,41 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9252720" y="325440"/>
-          <a:ext cx="0" cy="975240"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="18000">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>52560</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>218160</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+        <a:xfrm>
+          <a:off x="9484200" y="326160"/>
+          <a:ext cx="6120" cy="966600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>6480</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1237,9 +1250,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9252720" y="1308600"/>
-          <a:ext cx="0" cy="975240"/>
+        <a:xfrm>
+          <a:off x="9484200" y="1308600"/>
+          <a:ext cx="6120" cy="966600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1268,15 +1281,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1285,7 +1298,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4190040" y="325080"/>
+          <a:off x="4736880" y="325440"/>
           <a:ext cx="0" cy="969480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1316,7 +1329,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>248400</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1327,8 +1340,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5265720" y="325080"/>
-          <a:ext cx="521280" cy="0"/>
+          <a:off x="5814360" y="325080"/>
+          <a:ext cx="522720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1358,7 +1371,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>263880</xdr:colOff>
+      <xdr:colOff>264240</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1369,8 +1382,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6616080" y="325080"/>
-          <a:ext cx="266400" cy="0"/>
+          <a:off x="7167960" y="325080"/>
+          <a:ext cx="267120" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1411,8 +1424,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7966440" y="1299240"/>
-          <a:ext cx="521280" cy="0"/>
+          <a:off x="8521560" y="1299240"/>
+          <a:ext cx="522720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1436,7 +1449,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>-360</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1453,8 +1466,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9316800" y="325080"/>
-          <a:ext cx="521280" cy="0"/>
+          <a:off x="9875880" y="325080"/>
+          <a:ext cx="521640" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1478,7 +1491,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>153720</xdr:rowOff>
     </xdr:from>
@@ -1495,8 +1508,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4190040" y="1299240"/>
-          <a:ext cx="2962440" cy="0"/>
+          <a:off x="4736880" y="1299240"/>
+          <a:ext cx="2968920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1520,13 +1533,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>-360</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>153720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>266040</xdr:colOff>
+      <xdr:colOff>266400</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
@@ -1537,7 +1550,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9316800" y="1299240"/>
+          <a:off x="9875880" y="1299240"/>
           <a:ext cx="266400" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1562,13 +1575,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>-360</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>153720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>258840</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
@@ -1579,7 +1592,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9316800" y="1299240"/>
+          <a:off x="9875880" y="1299240"/>
           <a:ext cx="258840" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1610,7 +1623,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1621,8 +1634,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3915720" y="325080"/>
-          <a:ext cx="521280" cy="0"/>
+          <a:off x="4461480" y="325080"/>
+          <a:ext cx="522360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1646,15 +1659,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>267840</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>267840</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1663,7 +1676,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6886080" y="325440"/>
+          <a:off x="7438680" y="325800"/>
           <a:ext cx="0" cy="969480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1690,13 +1703,13 @@
       <xdr:col>32</xdr:col>
       <xdr:colOff>-360</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>-360</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1705,49 +1718,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9586800" y="325440"/>
-          <a:ext cx="0" cy="969480"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="18000">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8236440" y="325440"/>
+          <a:off x="10146240" y="325800"/>
           <a:ext cx="0" cy="969480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1773,6 +1744,48 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>268920</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>268920</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>150120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8792280" y="325800"/>
+          <a:ext cx="0" cy="969480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>269280</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1789,8 +1802,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8236800" y="325080"/>
-          <a:ext cx="258840" cy="0"/>
+          <a:off x="8792640" y="325080"/>
+          <a:ext cx="259560" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1822,553 +1835,619 @@
   <dimension ref="A1:AK16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="3.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="1" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="5" t="n">
+      <c r="O1" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="7" t="n">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="9" t="n">
         <f aca="false">O1+O3</f>
         <v>6</v>
       </c>
-      <c r="T1" s="5" t="n">
+      <c r="T1" s="7" t="n">
         <f aca="false">Q1</f>
         <v>6</v>
       </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="7" t="n">
+      <c r="U1" s="8"/>
+      <c r="V1" s="9" t="n">
         <f aca="false">T1+T3</f>
-        <v>10</v>
-      </c>
-      <c r="AD1" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD1" s="7" t="n">
         <f aca="false">MAX(V1,AA7)</f>
+        <v>13</v>
+      </c>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="9" t="n">
+        <f aca="false">AD1+AD3</f>
         <v>14</v>
-      </c>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="7" t="n">
-        <f aca="false">AD1+AD3</f>
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="1" t="n">
+      <c r="G2" s="13"/>
+      <c r="H2" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="O2" s="12" t="s">
+      <c r="I2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <f aca="false">ROUND(H2/(I2*J2),0)</f>
+        <v>6</v>
+      </c>
+      <c r="O2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="T2" s="12" t="s">
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="T2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="AD2" s="12" t="s">
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="AD2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="11" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="1" t="n">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="O3" s="15" t="n">
-        <f aca="false">H2</f>
+      <c r="I3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <f aca="false">ROUND(H3/(I3*J3),0)</f>
+        <v>7</v>
+      </c>
+      <c r="O3" s="17" t="n">
+        <f aca="false">K2</f>
         <v>6</v>
       </c>
-      <c r="P3" s="16" t="n">
+      <c r="P3" s="18" t="n">
         <f aca="false">Q4-Q1</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="16" t="n">
+      <c r="Q3" s="18" t="n">
         <f aca="false">MIN(T1,T7,T13)-Q1</f>
         <v>0</v>
       </c>
-      <c r="T3" s="15" t="n">
-        <f aca="false">H3</f>
-        <v>4</v>
-      </c>
-      <c r="U3" s="16" t="n">
+      <c r="T3" s="17" t="n">
+        <f aca="false">K3</f>
+        <v>7</v>
+      </c>
+      <c r="U3" s="18" t="n">
         <f aca="false">V4-V1</f>
-        <v>4</v>
-      </c>
-      <c r="V3" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="18" t="n">
         <f aca="false">AD1-V1</f>
-        <v>4</v>
-      </c>
-      <c r="AD3" s="15" t="n">
-        <f aca="false">H8</f>
-        <v>1</v>
-      </c>
-      <c r="AE3" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="17" t="n">
+        <f aca="false">K8</f>
+        <v>1</v>
+      </c>
+      <c r="AE3" s="18" t="n">
         <f aca="false">AF4-AF1</f>
         <v>0</v>
       </c>
-      <c r="AF3" s="16" t="n">
+      <c r="AF3" s="18" t="n">
         <f aca="false">AI7-AF1</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="11" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="1" t="n">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="O4" s="17" t="n">
+      <c r="I4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <f aca="false">ROUND(H4/(I4*J4),0)</f>
+        <v>3</v>
+      </c>
+      <c r="O4" s="19" t="n">
         <f aca="false">Q4-O3</f>
         <v>0</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="18" t="n">
+      <c r="P4" s="8"/>
+      <c r="Q4" s="20" t="n">
         <f aca="false">MIN(T4,T10,T17)</f>
         <v>6</v>
       </c>
-      <c r="T4" s="17" t="n">
+      <c r="T4" s="19" t="n">
         <f aca="false">V4-T3</f>
-        <v>10</v>
-      </c>
-      <c r="U4" s="6"/>
-      <c r="V4" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="U4" s="8"/>
+      <c r="V4" s="20" t="n">
         <f aca="false">AD4</f>
+        <v>13</v>
+      </c>
+      <c r="AD4" s="19" t="n">
+        <f aca="false">AF4-AD3</f>
+        <v>13</v>
+      </c>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="20" t="n">
+        <f aca="false">AI10</f>
         <v>14</v>
-      </c>
-      <c r="AD4" s="17" t="n">
-        <f aca="false">AF4-AD3</f>
-        <v>14</v>
-      </c>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="18" t="n">
-        <f aca="false">AI10</f>
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="1" t="n">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="I5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <f aca="false">(100%+(100%-$J$3))/2</f>
+        <v>0.7</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <f aca="false">ROUND(H5/(I5*J5),0)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="11" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="1" t="n">
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="I6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <f aca="false">(100%+(100%-$J$3))/2</f>
+        <v>0.7</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <f aca="false">ROUND(H6/(I6*J6),0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="11" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="1" t="n">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="T7" s="5" t="n">
+      <c r="I7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <f aca="false">ROUND(H7/(I7*J7),0)</f>
+        <v>2</v>
+      </c>
+      <c r="T7" s="7" t="n">
         <f aca="false">Q1</f>
         <v>6</v>
       </c>
-      <c r="U7" s="6"/>
-      <c r="V7" s="7" t="n">
+      <c r="U7" s="8"/>
+      <c r="V7" s="9" t="n">
         <f aca="false">T7+T9</f>
+        <v>10</v>
+      </c>
+      <c r="Y7" s="7" t="n">
+        <f aca="false">V7</f>
+        <v>10</v>
+      </c>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="9" t="n">
+        <f aca="false">Y7+Y9</f>
         <v>12</v>
       </c>
-      <c r="Y7" s="5" t="n">
-        <f aca="false">V7</f>
-        <v>12</v>
-      </c>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="7" t="n">
-        <f aca="false">Y7+Y9</f>
+      <c r="AI7" s="7" t="n">
+        <f aca="false">MAX(AF1,AF13)</f>
         <v>14</v>
       </c>
-      <c r="AI7" s="5" t="n">
-        <f aca="false">MAX(AF1,AF13)</f>
-        <v>15</v>
-      </c>
-      <c r="AJ7" s="6"/>
-      <c r="AK7" s="7" t="n">
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="9" t="n">
         <f aca="false">AI7+AI9</f>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="T8" s="12" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <f aca="false">ROUND(H8/(I8*J8),0)</f>
+        <v>1</v>
+      </c>
+      <c r="T8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="Y8" s="12" t="s">
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="Y8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="12"/>
-      <c r="AI8" s="12" t="s">
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AI8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AJ8" s="12"/>
-      <c r="AK8" s="12"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="11" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="1" t="n">
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="T9" s="15" t="n">
-        <f aca="false">H5</f>
-        <v>6</v>
-      </c>
-      <c r="U9" s="16" t="n">
+      <c r="I9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <f aca="false">ROUND(H9/(I9*J9),0)</f>
+        <v>2</v>
+      </c>
+      <c r="T9" s="17" t="n">
+        <f aca="false">K5</f>
+        <v>4</v>
+      </c>
+      <c r="U9" s="18" t="n">
         <f aca="false">V10-V7</f>
-        <v>0</v>
-      </c>
-      <c r="V9" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="V9" s="18" t="n">
         <f aca="false">Y7-V7</f>
         <v>0</v>
       </c>
-      <c r="Y9" s="15" t="n">
-        <f aca="false">H7</f>
+      <c r="Y9" s="17" t="n">
+        <f aca="false">K7</f>
         <v>2</v>
       </c>
-      <c r="Z9" s="16" t="n">
+      <c r="Z9" s="18" t="n">
         <f aca="false">AA10-AA7</f>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="18" t="n">
         <f aca="false">AD1-AA7</f>
-        <v>0</v>
-      </c>
-      <c r="AI9" s="15" t="n">
-        <f aca="false">H10</f>
+        <v>1</v>
+      </c>
+      <c r="AI9" s="17" t="n">
+        <f aca="false">K10</f>
         <v>9</v>
       </c>
-      <c r="AJ9" s="16" t="n">
+      <c r="AJ9" s="18" t="n">
         <f aca="false">AK10-AK7</f>
         <v>0</v>
       </c>
-      <c r="AK9" s="16"/>
+      <c r="AK9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="1" t="n">
+      <c r="D10" s="16"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="T10" s="17" t="n">
+      <c r="I10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <f aca="false">ROUND(H10/(I10*J10),0)</f>
+        <v>9</v>
+      </c>
+      <c r="T10" s="19" t="n">
         <f aca="false">V10-T9</f>
-        <v>6</v>
-      </c>
-      <c r="U10" s="6"/>
-      <c r="V10" s="18" t="n">
+        <v>7</v>
+      </c>
+      <c r="U10" s="8"/>
+      <c r="V10" s="20" t="n">
         <f aca="false">Y10</f>
-        <v>12</v>
-      </c>
-      <c r="Y10" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y10" s="19" t="n">
         <f aca="false">AA10-Y9</f>
-        <v>12</v>
-      </c>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="20" t="n">
         <f aca="false">AD4</f>
+        <v>13</v>
+      </c>
+      <c r="AI10" s="19" t="n">
+        <f aca="false">AK10-AI9</f>
         <v>14</v>
       </c>
-      <c r="AI10" s="17" t="n">
-        <f aca="false">AK10-AI9</f>
-        <v>15</v>
-      </c>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="18" t="n">
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="20" t="n">
         <f aca="false">AK7</f>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T13" s="5" t="n">
+      <c r="T13" s="7" t="n">
         <f aca="false">Q1</f>
         <v>6</v>
       </c>
-      <c r="U13" s="6"/>
-      <c r="V13" s="7" t="n">
+      <c r="U13" s="8"/>
+      <c r="V13" s="9" t="n">
         <f aca="false">T13+T15</f>
         <v>9</v>
       </c>
-      <c r="Y13" s="5" t="n">
+      <c r="Y13" s="7" t="n">
         <f aca="false">V13</f>
         <v>9</v>
       </c>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="7" t="n">
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="9" t="n">
         <f aca="false">Y13+Y15</f>
-        <v>12</v>
-      </c>
-      <c r="AD13" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD13" s="7" t="n">
         <f aca="false">AA13</f>
-        <v>12</v>
-      </c>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="9" t="n">
         <f aca="false">AD13+AD15</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T14" s="12" t="s">
+      <c r="T14" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-      <c r="Y14" s="12" t="s">
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="Y14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
-      <c r="AD14" s="12" t="s">
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AD14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T15" s="15" t="n">
-        <f aca="false">H4</f>
+      <c r="T15" s="17" t="n">
+        <f aca="false">K4</f>
         <v>3</v>
       </c>
-      <c r="U15" s="16" t="n">
+      <c r="U15" s="18" t="n">
         <f aca="false">V16-V13</f>
         <v>1</v>
       </c>
-      <c r="V15" s="16" t="n">
+      <c r="V15" s="18" t="n">
         <f aca="false">Y13-V13</f>
         <v>0</v>
       </c>
-      <c r="Y15" s="15" t="n">
-        <f aca="false">H6</f>
-        <v>3</v>
-      </c>
-      <c r="Z15" s="16" t="n">
+      <c r="Y15" s="17" t="n">
+        <f aca="false">K6</f>
+        <v>2</v>
+      </c>
+      <c r="Z15" s="18" t="n">
         <f aca="false">AA16-AA13</f>
         <v>1</v>
       </c>
-      <c r="AA15" s="16" t="n">
+      <c r="AA15" s="18" t="n">
         <f aca="false">AD13-AA13</f>
         <v>0</v>
       </c>
-      <c r="AD15" s="15" t="n">
-        <f aca="false">H9</f>
+      <c r="AD15" s="17" t="n">
+        <f aca="false">K9</f>
         <v>2</v>
       </c>
-      <c r="AE15" s="16" t="n">
+      <c r="AE15" s="18" t="n">
         <f aca="false">AF16-AF13</f>
         <v>1</v>
       </c>
-      <c r="AF15" s="16" t="n">
+      <c r="AF15" s="18" t="n">
         <f aca="false">AI7-AF13</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T16" s="17" t="n">
+      <c r="T16" s="19" t="n">
         <f aca="false">V16-T15</f>
         <v>7</v>
       </c>
-      <c r="U16" s="6"/>
-      <c r="V16" s="18" t="n">
+      <c r="U16" s="8"/>
+      <c r="V16" s="20" t="n">
         <f aca="false">Y16</f>
         <v>10</v>
       </c>
-      <c r="Y16" s="17" t="n">
+      <c r="Y16" s="19" t="n">
         <f aca="false">AA16-Y15</f>
         <v>10</v>
       </c>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="18" t="n">
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="20" t="n">
         <f aca="false">AD16</f>
-        <v>13</v>
-      </c>
-      <c r="AD16" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD16" s="19" t="n">
         <f aca="false">AF16-AD15</f>
-        <v>13</v>
-      </c>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="20" t="n">
         <f aca="false">AI10</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2408,416 +2487,469 @@
   </sheetPr>
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="3.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="3.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="19" width="10.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="19" width="3.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="21" width="10.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="21" width="3.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="6.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="21" width="8.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="21" width="3.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="n">
+      <c r="I1" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7" t="n">
+      <c r="J1" s="8"/>
+      <c r="K1" s="9" t="n">
         <f aca="false">I1+I3</f>
-        <v>0</v>
-      </c>
-      <c r="N1" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="7" t="n">
         <f aca="false">K1</f>
-        <v>0</v>
-      </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="O1" s="8"/>
+      <c r="P1" s="9" t="n">
         <f aca="false">N1+N3</f>
-        <v>0</v>
-      </c>
-      <c r="S1" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="S1" s="7" t="n">
         <f aca="false">P1</f>
-        <v>0</v>
-      </c>
-      <c r="T1" s="6"/>
-      <c r="U1" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="T1" s="8"/>
+      <c r="U1" s="9" t="n">
         <f aca="false">S1+S3</f>
-        <v>0</v>
-      </c>
-      <c r="AC1" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="7" t="n">
         <f aca="false">Z7</f>
-        <v>0</v>
-      </c>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="9" t="n">
         <f aca="false">AC1+AC3</f>
-        <v>0</v>
-      </c>
-      <c r="AH1" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="7" t="n">
         <f aca="false">MAX(AE1,AE7)</f>
-        <v>0</v>
-      </c>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="9" t="n">
         <f aca="false">AH1+AH3</f>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
-      <c r="I2" s="12" t="s">
+      <c r="E2" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="30" t="n">
+        <f aca="false">ROUND(D2/(E2*F2),0)</f>
+        <v>3</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="N2" s="12" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="N2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="S2" s="12" t="s">
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="S2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="AC2" s="12" t="s">
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="AC2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AH2" s="12" t="s">
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AH2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="25" t="n">
+      <c r="D3" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25"/>
-      <c r="I3" s="15" t="n">
+      <c r="E3" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="30" t="n">
+        <f aca="false">ROUND(D3/(E3*F3),0)</f>
+        <v>4</v>
+      </c>
+      <c r="I3" s="17" t="n">
         <f aca="false">G2</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="18" t="n">
         <f aca="false">K4-K1</f>
         <v>0</v>
       </c>
-      <c r="K3" s="16" t="n">
+      <c r="K3" s="18" t="n">
         <f aca="false">MIN(X7,N1)-K1</f>
         <v>0</v>
       </c>
-      <c r="N3" s="15" t="n">
+      <c r="N3" s="17" t="n">
         <f aca="false">G3</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="O3" s="18" t="n">
         <f aca="false">P4-P1</f>
         <v>0</v>
       </c>
-      <c r="P3" s="16" t="n">
+      <c r="P3" s="18" t="n">
         <f aca="false">S1-P1</f>
         <v>0</v>
       </c>
-      <c r="S3" s="15" t="n">
+      <c r="S3" s="17" t="n">
         <f aca="false">G4</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" s="18" t="n">
         <f aca="false">U4-U1</f>
         <v>0</v>
       </c>
-      <c r="U3" s="16" t="n">
+      <c r="U3" s="18" t="n">
         <f aca="false">X7-U1</f>
         <v>0</v>
       </c>
-      <c r="AC3" s="15" t="n">
+      <c r="AC3" s="17" t="n">
         <f aca="false">G6</f>
-        <v>0</v>
-      </c>
-      <c r="AD3" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD3" s="18" t="n">
         <f aca="false">AE4-AE1</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="16" t="n">
+      <c r="AE3" s="18" t="n">
         <f aca="false">AH1-AE1</f>
         <v>0</v>
       </c>
-      <c r="AH3" s="15" t="n">
+      <c r="AH3" s="17" t="n">
         <f aca="false">G8</f>
-        <v>0</v>
-      </c>
-      <c r="AI3" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI3" s="18" t="n">
         <f aca="false">AJ4-AJ1</f>
         <v>0</v>
       </c>
-      <c r="AJ3" s="16"/>
+      <c r="AJ3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="25" t="n">
+      <c r="D4" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-      <c r="I4" s="17" t="n">
+      <c r="E4" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="30" t="n">
+        <f aca="false">ROUND(D4/(E4*F4),0)</f>
+        <v>3</v>
+      </c>
+      <c r="I4" s="19" t="n">
         <f aca="false">K4-I3</f>
         <v>0</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="18" t="n">
+      <c r="J4" s="8"/>
+      <c r="K4" s="20" t="n">
         <f aca="false">MIN(N4,X10)</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="N4" s="19" t="n">
         <f aca="false">P4-N3</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="O4" s="8"/>
+      <c r="P4" s="20" t="n">
         <f aca="false">S4</f>
-        <v>0</v>
-      </c>
-      <c r="S4" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="S4" s="19" t="n">
         <f aca="false">U4-S3</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="6"/>
-      <c r="U4" s="18" t="n">
+        <v>7</v>
+      </c>
+      <c r="T4" s="8"/>
+      <c r="U4" s="20" t="n">
         <f aca="false">X10</f>
-        <v>0</v>
-      </c>
-      <c r="AC4" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="19" t="n">
         <f aca="false">AE4-AC3</f>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="20" t="n">
         <f aca="false">AH4</f>
-        <v>0</v>
-      </c>
-      <c r="AH4" s="17" t="n">
+        <v>18</v>
+      </c>
+      <c r="AH4" s="19" t="n">
         <f aca="false">AJ4-AH3</f>
-        <v>0</v>
-      </c>
-      <c r="AI4" s="6"/>
-      <c r="AJ4" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="20" t="n">
         <f aca="false">AJ1</f>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="25" t="n">
+      <c r="D5" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
+      <c r="E5" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="30" t="n">
+        <f aca="false">ROUND(D5/(E5*F5),0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="25" t="n">
+      <c r="D6" s="30" t="n">
         <v>9</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="E6" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="29" t="n">
+        <f aca="false">(100%+(100%-F7))/2</f>
+        <v>0.75</v>
+      </c>
+      <c r="G6" s="30" t="n">
+        <f aca="false">ROUND(D6/(E6*F6),0)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="25" t="n">
+      <c r="D7" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
+      <c r="E7" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="30" t="n">
+        <f aca="false">ROUND(D7/(E7*F7),0)</f>
+        <v>4</v>
+      </c>
       <c r="N7" s="0"/>
       <c r="O7" s="0"/>
       <c r="P7" s="0"/>
-      <c r="X7" s="5" t="n">
+      <c r="X7" s="7" t="n">
         <f aca="false">MAX(K1,U1)</f>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="9" t="n">
         <f aca="false">X7+X9</f>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC7" s="7" t="n">
         <f aca="false">Z7</f>
-        <v>0</v>
-      </c>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="9" t="n">
         <f aca="false">AC7+AC9</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="26" t="n">
+      <c r="C8" s="32"/>
+      <c r="D8" s="31" t="n">
         <v>6</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="26"/>
+      <c r="E8" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="30" t="n">
+        <f aca="false">ROUND(D8/(E8*F8),0)</f>
+        <v>6</v>
+      </c>
       <c r="N8" s="0"/>
       <c r="O8" s="0"/>
       <c r="P8" s="0"/>
-      <c r="X8" s="12" t="s">
+      <c r="X8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
-      <c r="AC8" s="12" t="s">
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AC8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AD8" s="12"/>
-      <c r="AE8" s="12"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
+      <c r="F9" s="1"/>
       <c r="N9" s="0"/>
       <c r="O9" s="0"/>
       <c r="P9" s="0"/>
-      <c r="X9" s="15" t="n">
+      <c r="X9" s="17" t="n">
         <f aca="false">G5</f>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="18" t="n">
         <f aca="false">Z10-Z7</f>
         <v>0</v>
       </c>
-      <c r="Z9" s="16" t="n">
+      <c r="Z9" s="18" t="n">
         <f aca="false">MIN(AC1,AC7)-Z7</f>
         <v>0</v>
       </c>
-      <c r="AC9" s="15" t="n">
+      <c r="AC9" s="17" t="n">
         <f aca="false">G7</f>
-        <v>0</v>
-      </c>
-      <c r="AD9" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD9" s="18" t="n">
         <f aca="false">AE10-AE7</f>
-        <v>0</v>
-      </c>
-      <c r="AE9" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="18" t="n">
         <f aca="false">AH1-AE7</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
+      <c r="F10" s="1"/>
       <c r="N10" s="0"/>
       <c r="O10" s="0"/>
       <c r="P10" s="0"/>
-      <c r="X10" s="17" t="n">
+      <c r="X10" s="19" t="n">
         <f aca="false">Z10-X9</f>
-        <v>0</v>
-      </c>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="20" t="n">
         <f aca="false">MIN(AC4,AC10)</f>
-        <v>0</v>
-      </c>
-      <c r="AC10" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC10" s="19" t="n">
         <f aca="false">AE10-AC9</f>
-        <v>0</v>
-      </c>
-      <c r="AD10" s="6"/>
-      <c r="AE10" s="18" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="20" t="n">
         <f aca="false">AH4</f>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>